<commit_message>
gather fertilizer and energy data
</commit_message>
<xml_diff>
--- a/data/data_analysis/calcs.xlsx
+++ b/data/data_analysis/calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\data\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CBCEF4A-D7D6-4033-B38E-D364BE1112AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC9A523-228C-4144-B873-2739360B7582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{C7A76F81-B13B-4D78-BFBE-6D99FEBC3FCB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="100">
   <si>
     <t>SSP1</t>
   </si>
@@ -255,6 +255,87 @@
   </si>
   <si>
     <t>Unit</t>
+  </si>
+  <si>
+    <t>Non-Staples</t>
+  </si>
+  <si>
+    <t>Staples</t>
+  </si>
+  <si>
+    <t>USD$/Mcal/day</t>
+  </si>
+  <si>
+    <t>Change in food prices</t>
+  </si>
+  <si>
+    <t>Food Sector Carbon Emissions in 2050</t>
+  </si>
+  <si>
+    <t>CO2-Ceq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GWP of methane: </t>
+  </si>
+  <si>
+    <t>Methane C avoidance</t>
+  </si>
+  <si>
+    <t>Carbon Sequestration</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>[Almaraz et al., 2023]</t>
+  </si>
+  <si>
+    <t>Food system emissions in 2050 (Gt CO2-eq)</t>
+  </si>
+  <si>
+    <t>Food system emissions in 2050 (Mt C)</t>
+  </si>
+  <si>
+    <t>Percentage reduction</t>
+  </si>
+  <si>
+    <t>fuel</t>
+  </si>
+  <si>
+    <t>oil</t>
+  </si>
+  <si>
+    <t>EJ</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>nuclear</t>
+  </si>
+  <si>
+    <t>hydro</t>
+  </si>
+  <si>
+    <t>wind</t>
+  </si>
+  <si>
+    <t>solar</t>
+  </si>
+  <si>
+    <t>geothermal</t>
+  </si>
+  <si>
+    <t>traditional biomass</t>
+  </si>
+  <si>
+    <t>natural gas</t>
+  </si>
+  <si>
+    <t>Energy sector changes</t>
   </si>
 </sst>
 </file>
@@ -626,16 +707,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79C2F0F-B8AA-4DA1-8F6F-DAD668A995C1}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:Z130"/>
+  <dimension ref="A1:AE130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AC16" sqref="AC16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -648,8 +728,20 @@
       <c r="W1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AC1">
+        <v>2050</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>2050</v>
       </c>
@@ -704,8 +796,20 @@
       <c r="Z2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC2">
+        <v>3.4622E-2</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>26</v>
       </c>
@@ -757,8 +861,20 @@
       <c r="Z3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB3" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC3">
+        <v>-2.542E-3</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>27</v>
       </c>
@@ -816,8 +932,20 @@
       <c r="Z4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC4">
+        <v>13.283339</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>28</v>
       </c>
@@ -875,8 +1003,20 @@
       <c r="Z5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC5">
+        <v>-2.7608220000000001</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>29</v>
       </c>
@@ -935,7 +1075,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>
@@ -1003,7 +1143,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>339</v>
       </c>
@@ -1056,7 +1196,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>340</v>
       </c>
@@ -1112,7 +1252,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>341</v>
       </c>
@@ -1168,7 +1308,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>342</v>
       </c>
@@ -1224,7 +1364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>343</v>
       </c>
@@ -1292,7 +1432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>652</v>
       </c>
@@ -1345,7 +1485,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>653</v>
       </c>
@@ -1404,7 +1544,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>654</v>
       </c>
@@ -1463,7 +1603,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>655</v>
       </c>
@@ -1680,6 +1820,21 @@
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="G21" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21">
+        <v>2050</v>
+      </c>
+      <c r="I21" t="s">
+        <v>87</v>
+      </c>
+      <c r="J21" t="s">
+        <v>23</v>
+      </c>
       <c r="M21">
         <v>64</v>
       </c>
@@ -1706,6 +1861,24 @@
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22">
+        <v>27.2</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>-5.4491880000000004</v>
+      </c>
+      <c r="I22" t="s">
+        <v>88</v>
+      </c>
+      <c r="J22" t="s">
+        <v>89</v>
+      </c>
       <c r="M22" t="s">
         <v>15</v>
       </c>
@@ -1744,6 +1917,25 @@
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23">
+        <f>12/44</f>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>-13.864243</v>
+      </c>
+      <c r="I23" t="s">
+        <v>98</v>
+      </c>
+      <c r="J23" t="s">
+        <v>89</v>
+      </c>
       <c r="N23" t="s">
         <v>28</v>
       </c>
@@ -1767,6 +1959,25 @@
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B24">
+        <f>H18*B22*B23</f>
+        <v>410.30000727272721</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>-15.926671000000001</v>
+      </c>
+      <c r="I24" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" t="s">
+        <v>89</v>
+      </c>
       <c r="M24">
         <v>0</v>
       </c>
@@ -1796,6 +2007,25 @@
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25">
+        <f>B18</f>
+        <v>142.86778999999999</v>
+      </c>
+      <c r="G25">
+        <v>3</v>
+      </c>
+      <c r="H25">
+        <v>-5.265949</v>
+      </c>
+      <c r="I25" t="s">
+        <v>91</v>
+      </c>
+      <c r="J25" t="s">
+        <v>89</v>
+      </c>
       <c r="M25">
         <v>32</v>
       </c>
@@ -1825,6 +2055,25 @@
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>82</v>
+      </c>
+      <c r="B26">
+        <f>B24+B25</f>
+        <v>553.16779727272717</v>
+      </c>
+      <c r="G26">
+        <v>4</v>
+      </c>
+      <c r="H26">
+        <v>5.1054760000000003</v>
+      </c>
+      <c r="I26" t="s">
+        <v>92</v>
+      </c>
+      <c r="J26" t="s">
+        <v>89</v>
+      </c>
       <c r="M26">
         <v>64</v>
       </c>
@@ -1854,6 +2103,18 @@
       </c>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>5</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>93</v>
+      </c>
+      <c r="J27" t="s">
+        <v>89</v>
+      </c>
       <c r="M27" t="s">
         <v>25</v>
       </c>
@@ -1892,6 +2153,27 @@
       </c>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28">
+        <v>5.7040009999999999</v>
+      </c>
+      <c r="I28" t="s">
+        <v>94</v>
+      </c>
+      <c r="J28" t="s">
+        <v>89</v>
+      </c>
       <c r="N28" t="s">
         <v>28</v>
       </c>
@@ -1915,6 +2197,25 @@
       </c>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29">
+        <f>B28*1000*B23</f>
+        <v>5018.181818181818</v>
+      </c>
+      <c r="G29">
+        <v>7</v>
+      </c>
+      <c r="H29">
+        <v>5.8336079999999999</v>
+      </c>
+      <c r="I29" t="s">
+        <v>95</v>
+      </c>
+      <c r="J29" t="s">
+        <v>89</v>
+      </c>
       <c r="M29">
         <v>0</v>
       </c>
@@ -1941,6 +2242,25 @@
       </c>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="B30">
+        <f>100*B26/B29</f>
+        <v>11.023271322463767</v>
+      </c>
+      <c r="G30">
+        <v>8</v>
+      </c>
+      <c r="H30">
+        <v>0.59675599999999995</v>
+      </c>
+      <c r="I30" t="s">
+        <v>96</v>
+      </c>
+      <c r="J30" t="s">
+        <v>89</v>
+      </c>
       <c r="M30">
         <v>32</v>
       </c>
@@ -1967,6 +2287,18 @@
       </c>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <v>9</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" t="s">
+        <v>97</v>
+      </c>
+      <c r="J31" t="s">
+        <v>89</v>
+      </c>
       <c r="M31">
         <v>64</v>
       </c>
@@ -1993,6 +2325,15 @@
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="H32">
+        <v>2050</v>
+      </c>
+      <c r="I32" t="s">
+        <v>87</v>
+      </c>
+      <c r="J32" t="s">
+        <v>23</v>
+      </c>
       <c r="M32" t="s">
         <v>15</v>
       </c>
@@ -2030,7 +2371,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="13:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>-3.3497110000000001</v>
+      </c>
+      <c r="I33" t="s">
+        <v>88</v>
+      </c>
+      <c r="J33" t="s">
+        <v>26</v>
+      </c>
       <c r="N33" t="s">
         <v>29</v>
       </c>
@@ -2053,7 +2406,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="13:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>-8.3438630000000007</v>
+      </c>
+      <c r="I34" t="s">
+        <v>98</v>
+      </c>
+      <c r="J34" t="s">
+        <v>26</v>
+      </c>
       <c r="M34">
         <v>0</v>
       </c>
@@ -2082,7 +2447,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>-25.941690000000001</v>
+      </c>
+      <c r="I35" t="s">
+        <v>90</v>
+      </c>
+      <c r="J35" t="s">
+        <v>26</v>
+      </c>
       <c r="M35">
         <v>32</v>
       </c>
@@ -2111,7 +2488,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <v>3</v>
+      </c>
+      <c r="H36">
+        <v>-2.9056890000000002</v>
+      </c>
+      <c r="I36" t="s">
+        <v>91</v>
+      </c>
+      <c r="J36" t="s">
+        <v>26</v>
+      </c>
       <c r="M36">
         <v>64</v>
       </c>
@@ -2140,7 +2529,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>15.637447</v>
+      </c>
+      <c r="I37" t="s">
+        <v>92</v>
+      </c>
+      <c r="J37" t="s">
+        <v>26</v>
+      </c>
       <c r="M37" t="s">
         <v>25</v>
       </c>
@@ -2178,7 +2579,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <v>5</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" t="s">
+        <v>93</v>
+      </c>
+      <c r="J38" t="s">
+        <v>26</v>
+      </c>
       <c r="N38" t="s">
         <v>29</v>
       </c>
@@ -2201,7 +2614,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <v>6</v>
+      </c>
+      <c r="H39">
+        <v>7.5080799999999996</v>
+      </c>
+      <c r="I39" t="s">
+        <v>94</v>
+      </c>
+      <c r="J39" t="s">
+        <v>26</v>
+      </c>
       <c r="M39">
         <v>0</v>
       </c>
@@ -2227,7 +2652,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40">
+        <v>6.3713490000000004</v>
+      </c>
+      <c r="I40" t="s">
+        <v>95</v>
+      </c>
+      <c r="J40" t="s">
+        <v>26</v>
+      </c>
       <c r="M40">
         <v>32</v>
       </c>
@@ -2253,7 +2690,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <v>8</v>
+      </c>
+      <c r="H41">
+        <v>7.7592090000000002</v>
+      </c>
+      <c r="I41" t="s">
+        <v>96</v>
+      </c>
+      <c r="J41" t="s">
+        <v>26</v>
+      </c>
       <c r="M41">
         <v>64</v>
       </c>
@@ -2279,7 +2728,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="7:26" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <v>9</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42" t="s">
+        <v>97</v>
+      </c>
+      <c r="J42" t="s">
+        <v>26</v>
+      </c>
       <c r="M42" t="s">
         <v>15</v>
       </c>
@@ -2317,7 +2778,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="7:26" x14ac:dyDescent="0.25">
       <c r="N43" t="s">
         <v>30</v>
       </c>
@@ -2340,7 +2801,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="7:26" x14ac:dyDescent="0.25">
       <c r="M44">
         <v>0</v>
       </c>
@@ -2369,7 +2830,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="7:26" x14ac:dyDescent="0.25">
       <c r="M45">
         <v>32</v>
       </c>
@@ -2398,7 +2859,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="7:26" x14ac:dyDescent="0.25">
       <c r="M46">
         <v>64</v>
       </c>
@@ -2427,7 +2888,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="7:26" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
         <v>25</v>
       </c>
@@ -2465,7 +2926,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="7:26" x14ac:dyDescent="0.25">
       <c r="N48" t="s">
         <v>30</v>
       </c>
@@ -2488,7 +2949,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="13:26" x14ac:dyDescent="0.25">
       <c r="M49">
         <v>0</v>
       </c>
@@ -2514,7 +2975,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="50" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="13:26" x14ac:dyDescent="0.25">
       <c r="M50">
         <v>32</v>
       </c>
@@ -2540,7 +3001,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="51" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="13:26" x14ac:dyDescent="0.25">
       <c r="M51">
         <v>64</v>
       </c>
@@ -2566,7 +3027,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W52" t="s">
         <v>66</v>
       </c>
@@ -2580,7 +3041,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="53" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W53" t="s">
         <v>66</v>
       </c>
@@ -2594,7 +3055,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W54" t="s">
         <v>66</v>
       </c>
@@ -2608,7 +3069,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="55" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W55" t="s">
         <v>66</v>
       </c>
@@ -2622,7 +3083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W56" t="s">
         <v>66</v>
       </c>
@@ -2636,7 +3097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W57" t="s">
         <v>66</v>
       </c>
@@ -2650,7 +3111,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="58" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W58" t="s">
         <v>66</v>
       </c>
@@ -2664,7 +3125,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W59" t="s">
         <v>66</v>
       </c>
@@ -2678,7 +3139,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="60" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W60" t="s">
         <v>66</v>
       </c>
@@ -2692,7 +3153,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W61" t="s">
         <v>66</v>
       </c>
@@ -2706,7 +3167,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W62" t="s">
         <v>66</v>
       </c>
@@ -2720,7 +3181,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W63" t="s">
         <v>66</v>
       </c>
@@ -2734,7 +3195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="13:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="13:26" x14ac:dyDescent="0.25">
       <c r="W64" t="s">
         <v>66</v>
       </c>
@@ -2748,7 +3209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W65" t="s">
         <v>66</v>
       </c>
@@ -2762,7 +3223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W66" t="s">
         <v>66</v>
       </c>
@@ -2776,7 +3237,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W67" t="s">
         <v>67</v>
       </c>
@@ -2790,7 +3251,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W68" t="s">
         <v>67</v>
       </c>
@@ -2804,7 +3265,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W69" t="s">
         <v>67</v>
       </c>
@@ -2818,7 +3279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W70" t="s">
         <v>67</v>
       </c>
@@ -2832,7 +3293,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W71" t="s">
         <v>67</v>
       </c>
@@ -2846,7 +3307,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W72" t="s">
         <v>67</v>
       </c>
@@ -2860,7 +3321,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W73" t="s">
         <v>67</v>
       </c>
@@ -2874,7 +3335,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W74" t="s">
         <v>67</v>
       </c>
@@ -2888,7 +3349,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W75" t="s">
         <v>67</v>
       </c>
@@ -2902,7 +3363,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W76" t="s">
         <v>67</v>
       </c>
@@ -2916,7 +3377,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W77" t="s">
         <v>67</v>
       </c>
@@ -2930,7 +3391,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W78" t="s">
         <v>67</v>
       </c>
@@ -2944,7 +3405,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W79" t="s">
         <v>67</v>
       </c>
@@ -2958,7 +3419,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W80" t="s">
         <v>67</v>
       </c>
@@ -2972,7 +3433,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W81" t="s">
         <v>67</v>
       </c>
@@ -2986,7 +3447,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W82" t="s">
         <v>67</v>
       </c>
@@ -3000,7 +3461,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W83" t="s">
         <v>67</v>
       </c>
@@ -3014,7 +3475,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W84" t="s">
         <v>67</v>
       </c>
@@ -3028,7 +3489,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W85" t="s">
         <v>67</v>
       </c>
@@ -3042,7 +3503,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W86" t="s">
         <v>67</v>
       </c>
@@ -3056,7 +3517,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W87" t="s">
         <v>67</v>
       </c>
@@ -3070,7 +3531,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W88" t="s">
         <v>67</v>
       </c>
@@ -3084,7 +3545,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W89" t="s">
         <v>67</v>
       </c>
@@ -3098,7 +3559,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W90" t="s">
         <v>67</v>
       </c>
@@ -3112,7 +3573,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W91" t="s">
         <v>67</v>
       </c>
@@ -3126,7 +3587,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W92" t="s">
         <v>67</v>
       </c>
@@ -3140,7 +3601,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W93" t="s">
         <v>67</v>
       </c>
@@ -3154,7 +3615,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W94" t="s">
         <v>67</v>
       </c>
@@ -3168,7 +3629,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W95" t="s">
         <v>67</v>
       </c>
@@ -3182,7 +3643,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W96" t="s">
         <v>67</v>
       </c>
@@ -3196,7 +3657,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W97" t="s">
         <v>67</v>
       </c>
@@ -3210,7 +3671,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W98" t="s">
         <v>67</v>
       </c>
@@ -3224,7 +3685,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W99" t="s">
         <v>68</v>
       </c>
@@ -3238,7 +3699,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W100" t="s">
         <v>68</v>
       </c>
@@ -3252,7 +3713,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W101" t="s">
         <v>68</v>
       </c>
@@ -3266,7 +3727,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W102" t="s">
         <v>68</v>
       </c>
@@ -3280,7 +3741,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W103" t="s">
         <v>68</v>
       </c>
@@ -3294,7 +3755,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W104" t="s">
         <v>68</v>
       </c>
@@ -3308,7 +3769,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W105" t="s">
         <v>68</v>
       </c>
@@ -3322,7 +3783,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W106" t="s">
         <v>68</v>
       </c>
@@ -3336,7 +3797,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W107" t="s">
         <v>68</v>
       </c>
@@ -3350,7 +3811,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W108" t="s">
         <v>68</v>
       </c>
@@ -3364,7 +3825,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W109" t="s">
         <v>68</v>
       </c>
@@ -3378,7 +3839,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W110" t="s">
         <v>68</v>
       </c>
@@ -3392,7 +3853,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W111" t="s">
         <v>68</v>
       </c>
@@ -3406,7 +3867,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W112" t="s">
         <v>68</v>
       </c>
@@ -3420,7 +3881,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W113" t="s">
         <v>68</v>
       </c>
@@ -3434,7 +3895,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W114" t="s">
         <v>68</v>
       </c>
@@ -3448,7 +3909,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W115" t="s">
         <v>68</v>
       </c>
@@ -3462,7 +3923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W116" t="s">
         <v>68</v>
       </c>
@@ -3476,7 +3937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W117" t="s">
         <v>68</v>
       </c>
@@ -3490,7 +3951,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W118" t="s">
         <v>68</v>
       </c>
@@ -3504,7 +3965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W119" t="s">
         <v>68</v>
       </c>
@@ -3518,7 +3979,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W120" t="s">
         <v>68</v>
       </c>
@@ -3532,7 +3993,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W121" t="s">
         <v>68</v>
       </c>
@@ -3546,7 +4007,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W122" t="s">
         <v>68</v>
       </c>
@@ -3560,7 +4021,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W123" t="s">
         <v>68</v>
       </c>
@@ -3574,7 +4035,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W124" t="s">
         <v>68</v>
       </c>
@@ -3588,7 +4049,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W125" t="s">
         <v>68</v>
       </c>
@@ -3602,7 +4063,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W126" t="s">
         <v>68</v>
       </c>
@@ -3616,7 +4077,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W127" t="s">
         <v>68</v>
       </c>
@@ -3630,7 +4091,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W128" t="s">
         <v>68</v>
       </c>
@@ -3644,7 +4105,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W129" t="s">
         <v>68</v>
       </c>
@@ -3658,7 +4119,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="23:26" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="23:26" x14ac:dyDescent="0.25">
       <c r="W130" t="s">
         <v>68</v>
       </c>
@@ -3674,11 +4135,6 @@
     </row>
   </sheetData>
   <autoFilter ref="W2:Z130" xr:uid="{F79C2F0F-B8AA-4DA1-8F6F-DAD668A995C1}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Biochar Application:&lt;br&gt;1.9632e+06 km&lt;sup&gt;2&lt;/sup&gt;"/>
-      </filters>
-    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="W3:Z34">
       <sortCondition descending="1" ref="Y2:Y130"/>
     </sortState>

</xml_diff>

<commit_message>
biochar decarbonization on a mass basis
</commit_message>
<xml_diff>
--- a/data/data_analysis/calcs.xlsx
+++ b/data/data_analysis/calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\data\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DC9A523-228C-4144-B873-2739360B7582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F788D6-F838-44EE-A82F-7FA2838701D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{C7A76F81-B13B-4D78-BFBE-6D99FEBC3FCB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="105">
   <si>
     <t>SSP1</t>
   </si>
@@ -278,15 +278,6 @@
     <t xml:space="preserve">GWP of methane: </t>
   </si>
   <si>
-    <t>Methane C avoidance</t>
-  </si>
-  <si>
-    <t>Carbon Sequestration</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>[Almaraz et al., 2023]</t>
   </si>
   <si>
@@ -336,6 +327,30 @@
   </si>
   <si>
     <t>Energy sector changes</t>
+  </si>
+  <si>
+    <t>Methane C avoidance (Mt C)</t>
+  </si>
+  <si>
+    <t>Carbon Sequestration (Mt C)</t>
+  </si>
+  <si>
+    <t>Total (Mt C)</t>
+  </si>
+  <si>
+    <t>Biochar Supply</t>
+  </si>
+  <si>
+    <t>Mt</t>
+  </si>
+  <si>
+    <t>Biochar Methane CO2-eq</t>
+  </si>
+  <si>
+    <t>Biochar Sequestration CO2-eq</t>
+  </si>
+  <si>
+    <t>Biochar total CO2-eq</t>
   </si>
 </sst>
 </file>
@@ -710,7 +725,7 @@
   <dimension ref="A1:AE130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1824,13 +1839,13 @@
         <v>77</v>
       </c>
       <c r="G21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="H21">
         <v>2050</v>
       </c>
       <c r="I21" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J21" t="s">
         <v>23</v>
@@ -1874,10 +1889,10 @@
         <v>-5.4491880000000004</v>
       </c>
       <c r="I22" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J22" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M22" t="s">
         <v>15</v>
@@ -1931,10 +1946,10 @@
         <v>-13.864243</v>
       </c>
       <c r="I23" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="N23" t="s">
         <v>28</v>
@@ -1960,7 +1975,7 @@
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="B24">
         <f>H18*B22*B23</f>
@@ -1973,10 +1988,10 @@
         <v>-15.926671000000001</v>
       </c>
       <c r="I24" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -2008,7 +2023,7 @@
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B25">
         <f>B18</f>
@@ -2021,10 +2036,10 @@
         <v>-5.265949</v>
       </c>
       <c r="I25" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M25">
         <v>32</v>
@@ -2056,7 +2071,7 @@
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B26">
         <f>B24+B25</f>
@@ -2069,10 +2084,10 @@
         <v>5.1054760000000003</v>
       </c>
       <c r="I26" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M26">
         <v>64</v>
@@ -2110,10 +2125,10 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M27" t="s">
         <v>25</v>
@@ -2154,13 +2169,13 @@
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B28">
         <v>18.399999999999999</v>
       </c>
       <c r="C28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="G28">
         <v>6</v>
@@ -2169,10 +2184,10 @@
         <v>5.7040009999999999</v>
       </c>
       <c r="I28" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="N28" t="s">
         <v>28</v>
@@ -2198,7 +2213,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B29">
         <f>B28*1000*B23</f>
@@ -2211,10 +2226,10 @@
         <v>5.8336079999999999</v>
       </c>
       <c r="I29" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -2243,7 +2258,7 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B30">
         <f>100*B26/B29</f>
@@ -2256,10 +2271,10 @@
         <v>0.59675599999999995</v>
       </c>
       <c r="I30" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J30" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M30">
         <v>32</v>
@@ -2294,10 +2309,10 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M31">
         <v>64</v>
@@ -2325,11 +2340,20 @@
       </c>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32">
+        <v>556.318579</v>
+      </c>
+      <c r="C32" t="s">
+        <v>101</v>
+      </c>
       <c r="H32">
         <v>2050</v>
       </c>
       <c r="I32" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J32" t="s">
         <v>23</v>
@@ -2371,7 +2395,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>102</v>
+      </c>
+      <c r="B33">
+        <f>H18*B22</f>
+        <v>1504.43336</v>
+      </c>
       <c r="G33">
         <v>0</v>
       </c>
@@ -2379,7 +2410,7 @@
         <v>-3.3497110000000001</v>
       </c>
       <c r="I33" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J33" t="s">
         <v>26</v>
@@ -2406,7 +2437,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>103</v>
+      </c>
+      <c r="B34">
+        <f>B25</f>
+        <v>142.86778999999999</v>
+      </c>
       <c r="G34">
         <v>1</v>
       </c>
@@ -2414,7 +2452,7 @@
         <v>-8.3438630000000007</v>
       </c>
       <c r="I34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="J34" t="s">
         <v>26</v>
@@ -2447,7 +2485,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B35">
+        <f>(B33+B34)/B32</f>
+        <v>2.9610752043569626</v>
+      </c>
       <c r="G35">
         <v>2</v>
       </c>
@@ -2455,7 +2500,7 @@
         <v>-25.941690000000001</v>
       </c>
       <c r="I35" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J35" t="s">
         <v>26</v>
@@ -2488,7 +2533,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="36" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G36">
         <v>3</v>
       </c>
@@ -2496,7 +2541,7 @@
         <v>-2.9056890000000002</v>
       </c>
       <c r="I36" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="J36" t="s">
         <v>26</v>
@@ -2529,7 +2574,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G37">
         <v>4</v>
       </c>
@@ -2537,7 +2582,7 @@
         <v>15.637447</v>
       </c>
       <c r="I37" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="J37" t="s">
         <v>26</v>
@@ -2579,7 +2624,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="38" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G38">
         <v>5</v>
       </c>
@@ -2587,7 +2632,7 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="J38" t="s">
         <v>26</v>
@@ -2614,7 +2659,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G39">
         <v>6</v>
       </c>
@@ -2622,7 +2667,7 @@
         <v>7.5080799999999996</v>
       </c>
       <c r="I39" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="J39" t="s">
         <v>26</v>
@@ -2652,7 +2697,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G40">
         <v>7</v>
       </c>
@@ -2660,7 +2705,7 @@
         <v>6.3713490000000004</v>
       </c>
       <c r="I40" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="J40" t="s">
         <v>26</v>
@@ -2690,7 +2735,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G41">
         <v>8</v>
       </c>
@@ -2698,7 +2743,7 @@
         <v>7.7592090000000002</v>
       </c>
       <c r="I41" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="J41" t="s">
         <v>26</v>
@@ -2728,7 +2773,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
       <c r="G42">
         <v>9</v>
       </c>
@@ -2736,7 +2781,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="J42" t="s">
         <v>26</v>
@@ -2778,7 +2823,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="43" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
       <c r="N43" t="s">
         <v>30</v>
       </c>
@@ -2801,7 +2846,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="44" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
       <c r="M44">
         <v>0</v>
       </c>
@@ -2830,7 +2875,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
       <c r="M45">
         <v>32</v>
       </c>
@@ -2859,7 +2904,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="46" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
       <c r="M46">
         <v>64</v>
       </c>
@@ -2888,7 +2933,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.25">
       <c r="M47" t="s">
         <v>25</v>
       </c>
@@ -2926,7 +2971,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="48" spans="7:26" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.25">
       <c r="N48" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
plotting food accessibility and found an error in dairy manure rates
</commit_message>
<xml_diff>
--- a/data/data_analysis/calcs.xlsx
+++ b/data/data_analysis/calcs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM\biochar\data\data_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9F788D6-F838-44EE-A82F-7FA2838701D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB55148C-B634-4F47-9C07-EE34040F0DCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{C7A76F81-B13B-4D78-BFBE-6D99FEBC3FCB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="801" uniqueCount="127">
   <si>
     <t>SSP1</t>
   </si>
@@ -351,6 +351,72 @@
   </si>
   <si>
     <t>Biochar total CO2-eq</t>
+  </si>
+  <si>
+    <t>LandLeaf</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>Feed</t>
+  </si>
+  <si>
+    <t>thousand</t>
+  </si>
+  <si>
+    <t>km$^2$</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>for</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Crops</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Grasslands</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Arable</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>Pasture</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>and</t>
+  </si>
+  <si>
+    <t>Desert</t>
+  </si>
+  <si>
+    <t>Shrubland</t>
+  </si>
+  <si>
+    <t>Tundra</t>
+  </si>
+  <si>
+    <t>Urban</t>
+  </si>
+  <si>
+    <t>Land for Food</t>
   </si>
 </sst>
 </file>
@@ -722,15 +788,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79C2F0F-B8AA-4DA1-8F6F-DAD668A995C1}">
-  <dimension ref="A1:AE130"/>
+  <dimension ref="A1:AH130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -756,7 +822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>2050</v>
       </c>
@@ -824,7 +890,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>26</v>
       </c>
@@ -889,7 +955,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>27</v>
       </c>
@@ -960,7 +1026,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>28</v>
       </c>
@@ -1031,7 +1097,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>29</v>
       </c>
@@ -1090,7 +1156,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>30</v>
       </c>
@@ -1158,7 +1224,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>339</v>
       </c>
@@ -1210,8 +1276,17 @@
       <c r="Z8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AC8">
+        <v>2050</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>340</v>
       </c>
@@ -1266,8 +1341,26 @@
       <c r="Z9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9">
+        <v>-42.537666999999999</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>108</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>341</v>
       </c>
@@ -1322,8 +1415,29 @@
       <c r="Z10" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AB10">
+        <v>1</v>
+      </c>
+      <c r="AC10">
+        <v>52.946877999999998</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>110</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>112</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>342</v>
       </c>
@@ -1378,8 +1492,23 @@
       <c r="Z11" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AB11">
+        <v>2</v>
+      </c>
+      <c r="AC11">
+        <v>-80.947716</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>343</v>
       </c>
@@ -1446,8 +1575,23 @@
       <c r="Z12" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AB12">
+        <v>3</v>
+      </c>
+      <c r="AC12">
+        <v>444.701007</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>114</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>652</v>
       </c>
@@ -1499,8 +1643,23 @@
       <c r="Z13" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AB13">
+        <v>4</v>
+      </c>
+      <c r="AC13">
+        <v>92.432309000000004</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>653</v>
       </c>
@@ -1558,8 +1717,29 @@
       <c r="Z14" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AB14">
+        <v>5</v>
+      </c>
+      <c r="AC14">
+        <v>-123.79096800000001</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>117</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>654</v>
       </c>
@@ -1617,8 +1797,23 @@
       <c r="Z15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="AB15">
+        <v>6</v>
+      </c>
+      <c r="AC15">
+        <v>-322.43952899999999</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>655</v>
       </c>
@@ -1676,8 +1871,29 @@
       <c r="Z16" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB16">
+        <v>7</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>120</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH16" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>656</v>
       </c>
@@ -1744,8 +1960,23 @@
       <c r="Z17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB17">
+        <v>8</v>
+      </c>
+      <c r="AC17">
+        <v>-20.365371</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>123</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -1781,8 +2012,23 @@
       <c r="Z18" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB18">
+        <v>9</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>124</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
       <c r="M19">
         <v>0</v>
       </c>
@@ -1807,8 +2053,23 @@
       <c r="Z19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB19">
+        <v>10</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>125</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>108</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
       <c r="M20">
         <v>32</v>
       </c>
@@ -1834,7 +2095,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -1875,7 +2136,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1930,8 +2191,15 @@
       <c r="Z22" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="AB22" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC22">
+        <f>AC9+AC11</f>
+        <v>-123.485383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -1973,7 +2241,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>97</v>
       </c>
@@ -2021,7 +2289,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -2069,7 +2337,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -2117,7 +2385,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G27">
         <v>5</v>
       </c>
@@ -2167,7 +2435,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>81</v>
       </c>
@@ -2211,7 +2479,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -2256,7 +2524,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>83</v>
       </c>
@@ -2301,7 +2569,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G31">
         <v>9</v>
       </c>
@@ -2339,7 +2607,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>100</v>
       </c>

</xml_diff>